<commit_message>
feat: Update MVP Plan
</commit_message>
<xml_diff>
--- a/project-2/Virus Tracker - Minimum Viable Product Plan.xlsx
+++ b/project-2/Virus Tracker - Minimum Viable Product Plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="140">
   <si>
     <r>
       <rPr>
@@ -388,6 +388,63 @@
     <t xml:space="preserve">-System notifies user by email
 -User can set number that stock must reach for email to be sent
 -System notifies user upon login that stock is low </t>
+  </si>
+  <si>
+    <t>report that I contracted the virus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) System confirms the report to the user by email 2) System explains to the user how to read general medical advices provided </t>
+  </si>
+  <si>
+    <t>read general advice written by professionals</t>
+  </si>
+  <si>
+    <t>I always have a medical reference about symptoms and potential cure / behavior to adopt</t>
+  </si>
+  <si>
+    <t>1) System allows to search for the symptoms 2) System provides a hotline number for emergencies</t>
+  </si>
+  <si>
+    <t>see the heat maps of the outbreak</t>
+  </si>
+  <si>
+    <t>new proactive strategies can be planned accordingly</t>
+  </si>
+  <si>
+    <t>1) User can search for town / area, System will show it on the map 2) System allows to zoom in / out</t>
+  </si>
+  <si>
+    <t>send funding to a specific area</t>
+  </si>
+  <si>
+    <t>funds can be used to stop the virus spreading in that area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) User can start the fund sending process directly from the heat maps report 2) User has a report page containing all the funds sent previously </t>
+  </si>
+  <si>
+    <t>report the number of death caused by the virus</t>
+  </si>
+  <si>
+    <t>1) User can report the number of death caused by virus 2) User can generate reports relate to the number of death caused by the virus for the previous months / years</t>
+  </si>
+  <si>
+    <t>write and update professional medical advice that will be available to patients</t>
+  </si>
+  <si>
+    <t>patience have a medical reference about symptoms and potential cure / behavior to adopt</t>
+  </si>
+  <si>
+    <t>1) User can create / delete / update the provided medical advice 2) User can check the previous version of a medical advice in the medical advice's history</t>
+  </si>
+  <si>
+    <t>report a change in the expected future production of tests</t>
+  </si>
+  <si>
+    <t>the CDC can take corrective actions in advance</t>
+  </si>
+  <si>
+    <t>1) Healthcare company can report a problem in production that can lead to a different number of test produced 2) Healthcare company can update the reported problem in case of change</t>
   </si>
   <si>
     <r>
@@ -770,7 +827,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -866,7 +923,6 @@
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1190,7 +1246,9 @@
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12"/>
       <c r="E3" s="13"/>
@@ -1201,7 +1259,9 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
+      <c r="D4" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="E4" s="13"/>
     </row>
     <row r="5">
@@ -1210,7 +1270,9 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
+      <c r="D5" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" s="13"/>
     </row>
     <row r="6">
@@ -1218,7 +1280,9 @@
         <v>9</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13"/>
     </row>
@@ -1229,7 +1293,9 @@
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
@@ -1238,13 +1304,17 @@
       <c r="B8" s="10"/>
       <c r="C8" s="14"/>
       <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
+      <c r="E8" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
@@ -1256,7 +1326,9 @@
       <c r="B10" s="17"/>
       <c r="C10" s="14"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
@@ -1264,14 +1336,18 @@
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
+      <c r="D11" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="E11" s="16"/>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
       <c r="E12" s="16"/>
@@ -1280,7 +1356,9 @@
       <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
@@ -1289,8 +1367,10 @@
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
     </row>
@@ -1300,8 +1380,10 @@
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
+      <c r="D15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="13"/>
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
@@ -1309,7 +1391,9 @@
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="E16" s="16"/>
     </row>
     <row r="17">
@@ -1317,7 +1401,9 @@
         <v>20</v>
       </c>
       <c r="B17" s="17"/>
-      <c r="C17" s="14"/>
+      <c r="C17" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16"/>
     </row>
@@ -1327,15 +1413,19 @@
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="17"/>
-      <c r="C19" s="14"/>
+      <c r="C19" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="D19" s="15"/>
       <c r="E19" s="16"/>
     </row>
@@ -1344,7 +1434,9 @@
         <v>23</v>
       </c>
       <c r="B20" s="17"/>
-      <c r="C20" s="14"/>
+      <c r="C20" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16"/>
     </row>
@@ -1352,7 +1444,9 @@
       <c r="A21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="C21" s="14"/>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
@@ -1364,7 +1458,9 @@
       <c r="B22" s="17"/>
       <c r="C22" s="14"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
+      <c r="E22" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1487,8 +1583,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="15.29"/>
-    <col customWidth="1" min="2" max="2" width="32.0"/>
-    <col customWidth="1" min="3" max="3" width="25.86"/>
+    <col customWidth="1" min="2" max="2" width="38.29"/>
+    <col customWidth="1" min="3" max="3" width="76.43"/>
     <col customWidth="1" min="4" max="4" width="45.57"/>
     <col customWidth="1" min="5" max="5" width="53.43"/>
   </cols>
@@ -1772,142 +1868,212 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="28"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
+      <c r="A17" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>93</v>
+      </c>
       <c r="D17" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
-      </c>
-      <c r="E17" s="32"/>
+        <v>As a Patient I can report that I contracted the virus so that data is accurate.</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="30"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
+      <c r="A18" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>101</v>
+      </c>
       <c r="D18" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
-      </c>
-      <c r="E18" s="33"/>
+        <v>As a Patient I can read general advice written by professionals so that I always have a medical reference about symptoms and potential cure / behavior to adopt.</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="30"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="A19" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>104</v>
+      </c>
       <c r="D19" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
-      </c>
-      <c r="E19" s="29"/>
+        <v>As a CDC Official I can see the heat maps of the outbreak so that new proactive strategies can be planned accordingly.</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="30"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>107</v>
+      </c>
       <c r="D20" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
-      </c>
-      <c r="E20" s="29"/>
+        <v>As a CDC Official I can send funding to a specific area so that funds can be used to stop the virus spreading in that area.</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="30"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>93</v>
+      </c>
       <c r="D21" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
-      </c>
-      <c r="E21" s="29"/>
+        <v>As a Doctor I can report the number of death caused by the virus so that data is accurate.</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="30"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="A22" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>112</v>
+      </c>
       <c r="D22" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
-      </c>
-      <c r="E22" s="29"/>
+        <v>As a Doctor I can write and update professional medical advice that will be available to patients so that patience have a medical reference about symptoms and potential cure / behavior to adopt.</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="30"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="A23" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>115</v>
+      </c>
       <c r="D23" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
-      </c>
-      <c r="E23" s="29"/>
+        <v>As a Healthcare Company I can report a change in the expected future production of tests so that the CDC can take corrective actions in advance.</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="30"/>
+      <c r="A24" s="28" t="s">
+        <v>63</v>
+      </c>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
       <c r="D24" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
+        <v>As a Healthcare Company I can  so that .</v>
       </c>
       <c r="E24" s="29"/>
     </row>
     <row r="25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
       <c r="D25" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
+        <v>As a Medical Examiner I can  so that .</v>
       </c>
       <c r="E25" s="29"/>
     </row>
     <row r="26">
-      <c r="A26" s="30"/>
+      <c r="A26" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="B26" s="28"/>
       <c r="C26" s="28"/>
       <c r="D26" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
+        <v>As a Medical Examiner I can  so that .</v>
       </c>
       <c r="E26" s="29"/>
     </row>
     <row r="27">
-      <c r="A27" s="30"/>
+      <c r="A27" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
+        <v>As a System Administrator I can  so that .</v>
       </c>
       <c r="E27" s="29"/>
     </row>
     <row r="28">
-      <c r="A28" s="30"/>
+      <c r="A28" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="B28" s="28"/>
       <c r="C28" s="28"/>
       <c r="D28" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
+        <v>As a System Administrator I can  so that .</v>
       </c>
       <c r="E28" s="29"/>
     </row>
     <row r="29">
-      <c r="A29" s="30"/>
+      <c r="A29" s="28" t="s">
+        <v>91</v>
+      </c>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
       <c r="D29" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
+        <v>As a Test Center I can  so that .</v>
       </c>
       <c r="E29" s="29"/>
     </row>
     <row r="30">
-      <c r="A30" s="30"/>
+      <c r="A30" s="28" t="s">
+        <v>91</v>
+      </c>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
       <c r="D30" s="28" t="str">
         <f t="shared" si="2"/>
-        <v>As a  I can  so that .</v>
+        <v>As a Test Center I can  so that .</v>
       </c>
       <c r="E30" s="29"/>
     </row>
@@ -2038,7 +2204,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="22" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2049,29 +2215,29 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>106</v>
+      <c r="A2" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3">
@@ -2089,20 +2255,20 @@
 -User can see a summary of the numbers provided
 -User must be logged in from a government IP address to view </v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40">
+      <c r="D3" s="38"/>
+      <c r="E3" s="39">
         <f>COUNTIF(D3:D39,"release 1-MVP")</f>
         <v>0</v>
       </c>
-      <c r="F3" s="41">
+      <c r="F3" s="40">
         <f>COUNTIF(D3:D39,"release 2")</f>
         <v>0</v>
       </c>
-      <c r="G3" s="41">
+      <c r="G3" s="40">
         <f>COUNTIF(D3:D39,"release 3")</f>
         <v>0</v>
       </c>
-      <c r="H3" s="41">
+      <c r="H3" s="40">
         <f>COUNTIF(D3:D39,"backlog for future release")</f>
         <v>0</v>
       </c>
@@ -2123,11 +2289,11 @@
 -User can see the names of the health care company
 -User can see amount of funds sent to each health care company</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="43"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="42"/>
     </row>
     <row r="5">
       <c r="A5" s="28" t="str">
@@ -2146,11 +2312,11 @@
 -Patient Location Required
 -Patient Gender is optional</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6">
       <c r="A6" s="28" t="str">
@@ -2166,11 +2332,11 @@
         <v>-User name and email address required
 -User is locked out after 3 incorrect entries</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
     </row>
     <row r="7">
       <c r="A7" s="28" t="str">
@@ -2187,11 +2353,11 @@
 -User can see data that previously entered
 </v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8">
       <c r="A8" s="28" t="str">
@@ -2207,11 +2373,11 @@
         <v>-User must verify email address
 -User must verify answer security question to reset password</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
     </row>
     <row r="9">
       <c r="A9" s="28" t="str">
@@ -2229,11 +2395,11 @@
 -Users gender selection is not shared with CDC Officials
 </v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
     </row>
     <row r="10">
       <c r="A10" s="28" t="str">
@@ -2249,11 +2415,11 @@
         <v>-Timeout occurs after 15 mins of inactivity
 -After timeout user is returned to login page</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
     </row>
     <row r="11">
       <c r="A11" s="28" t="str">
@@ -2269,11 +2435,11 @@
         <v>-User can modify test results twice
 -Doctors are notified when a patient changes test results</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
     </row>
     <row r="12">
       <c r="A12" s="28" t="str">
@@ -2289,11 +2455,11 @@
         <v>-Option only visible for patients that report positve test
 -Can specify store name, date entered, city, and state</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
     </row>
     <row r="13">
       <c r="A13" s="28" t="str">
@@ -2310,11 +2476,11 @@
 -Enter email addresses 
 -Gmail email address are not allowed access</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
     </row>
     <row r="14">
       <c r="A14" s="28" t="str">
@@ -2331,11 +2497,11 @@
 -Removed user can't login once removed
 -System administrator must confirm the user that they are removing before leaving the page</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
     </row>
     <row r="15">
       <c r="A15" s="28" t="str">
@@ -2351,11 +2517,11 @@
         <v>-Only allow update one time
 -Make user confirm change before leaving the page</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
     </row>
     <row r="16">
       <c r="A16" s="28" t="str">
@@ -2372,277 +2538,277 @@
 -User can set number that stock must reach for email to be sent
 -System notifies user upon login that stock is low </v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
     </row>
     <row r="17">
       <c r="A17" s="28" t="str">
         <f>'User Stories'!A17</f>
-        <v/>
+        <v>Patient</v>
       </c>
       <c r="B17" s="28" t="str">
         <f>'User Stories'!D17</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Patient I can report that I contracted the virus so that data is accurate.</v>
       </c>
       <c r="C17" s="28" t="str">
         <f>'User Stories'!E17</f>
-        <v/>
-      </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
+        <v>1) System confirms the report to the user by email 2) System explains to the user how to read general medical advices provided </v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
     </row>
     <row r="18">
       <c r="A18" s="28" t="str">
         <f>'User Stories'!A18</f>
-        <v/>
+        <v>Patient</v>
       </c>
       <c r="B18" s="28" t="str">
         <f>'User Stories'!D18</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Patient I can read general advice written by professionals so that I always have a medical reference about symptoms and potential cure / behavior to adopt.</v>
       </c>
       <c r="C18" s="28" t="str">
         <f>'User Stories'!E18</f>
-        <v/>
-      </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
+        <v>1) System allows to search for the symptoms 2) System provides a hotline number for emergencies</v>
+      </c>
+      <c r="D18" s="38"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
     </row>
     <row r="19">
       <c r="A19" s="28" t="str">
         <f>'User Stories'!A19</f>
-        <v/>
+        <v>CDC Official</v>
       </c>
       <c r="B19" s="28" t="str">
         <f>'User Stories'!D19</f>
-        <v>As a  I can  so that .</v>
+        <v>As a CDC Official I can see the heat maps of the outbreak so that new proactive strategies can be planned accordingly.</v>
       </c>
       <c r="C19" s="28" t="str">
         <f>'User Stories'!E19</f>
-        <v/>
-      </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
+        <v>1) User can search for town / area, System will show it on the map 2) System allows to zoom in / out</v>
+      </c>
+      <c r="D19" s="38"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
     </row>
     <row r="20">
       <c r="A20" s="28" t="str">
         <f>'User Stories'!A20</f>
-        <v/>
+        <v>CDC Official</v>
       </c>
       <c r="B20" s="28" t="str">
         <f>'User Stories'!D20</f>
-        <v>As a  I can  so that .</v>
+        <v>As a CDC Official I can send funding to a specific area so that funds can be used to stop the virus spreading in that area.</v>
       </c>
       <c r="C20" s="28" t="str">
         <f>'User Stories'!E20</f>
-        <v/>
-      </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
+        <v>1) User can start the fund sending process directly from the heat maps report 2) User has a report page containing all the funds sent previously </v>
+      </c>
+      <c r="D20" s="38"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
     </row>
     <row r="21">
       <c r="A21" s="28" t="str">
         <f>'User Stories'!A21</f>
-        <v/>
+        <v>Doctor</v>
       </c>
       <c r="B21" s="28" t="str">
         <f>'User Stories'!D21</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Doctor I can report the number of death caused by the virus so that data is accurate.</v>
       </c>
       <c r="C21" s="28" t="str">
         <f>'User Stories'!E21</f>
-        <v/>
-      </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
+        <v>1) User can report the number of death caused by virus 2) User can generate reports relate to the number of death caused by the virus for the previous months / years</v>
+      </c>
+      <c r="D21" s="38"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
     </row>
     <row r="22">
       <c r="A22" s="28" t="str">
         <f>'User Stories'!A22</f>
-        <v/>
+        <v>Doctor</v>
       </c>
       <c r="B22" s="28" t="str">
         <f>'User Stories'!D22</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Doctor I can write and update professional medical advice that will be available to patients so that patience have a medical reference about symptoms and potential cure / behavior to adopt.</v>
       </c>
       <c r="C22" s="28" t="str">
         <f>'User Stories'!E22</f>
-        <v/>
-      </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
+        <v>1) User can create / delete / update the provided medical advice 2) User can check the previous version of a medical advice in the medical advice's history</v>
+      </c>
+      <c r="D22" s="38"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
     </row>
     <row r="23">
       <c r="A23" s="28" t="str">
         <f>'User Stories'!A23</f>
-        <v/>
+        <v>Healthcare Company</v>
       </c>
       <c r="B23" s="28" t="str">
         <f>'User Stories'!D23</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Healthcare Company I can report a change in the expected future production of tests so that the CDC can take corrective actions in advance.</v>
       </c>
       <c r="C23" s="28" t="str">
         <f>'User Stories'!E23</f>
-        <v/>
-      </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
+        <v>1) Healthcare company can report a problem in production that can lead to a different number of test produced 2) Healthcare company can update the reported problem in case of change</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
     </row>
     <row r="24">
       <c r="A24" s="28" t="str">
         <f>'User Stories'!A24</f>
-        <v/>
+        <v>Healthcare Company</v>
       </c>
       <c r="B24" s="28" t="str">
         <f>'User Stories'!D24</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Healthcare Company I can  so that .</v>
       </c>
       <c r="C24" s="28" t="str">
         <f>'User Stories'!E24</f>
         <v/>
       </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
     </row>
     <row r="25">
       <c r="A25" s="28" t="str">
         <f>'User Stories'!A25</f>
-        <v/>
+        <v>Medical Examiner</v>
       </c>
       <c r="B25" s="28" t="str">
         <f>'User Stories'!D25</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Medical Examiner I can  so that .</v>
       </c>
       <c r="C25" s="28" t="str">
         <f>'User Stories'!E25</f>
         <v/>
       </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26">
       <c r="A26" s="28" t="str">
         <f>'User Stories'!A26</f>
-        <v/>
+        <v>Medical Examiner</v>
       </c>
       <c r="B26" s="28" t="str">
         <f>'User Stories'!D26</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Medical Examiner I can  so that .</v>
       </c>
       <c r="C26" s="28" t="str">
         <f>'User Stories'!E26</f>
         <v/>
       </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
     </row>
     <row r="27">
       <c r="A27" s="28" t="str">
         <f>'User Stories'!A27</f>
-        <v/>
+        <v>System Administrator</v>
       </c>
       <c r="B27" s="28" t="str">
         <f>'User Stories'!D27</f>
-        <v>As a  I can  so that .</v>
+        <v>As a System Administrator I can  so that .</v>
       </c>
       <c r="C27" s="28" t="str">
         <f>'User Stories'!E27</f>
         <v/>
       </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
     </row>
     <row r="28">
       <c r="A28" s="28" t="str">
         <f>'User Stories'!A28</f>
-        <v/>
+        <v>System Administrator</v>
       </c>
       <c r="B28" s="28" t="str">
         <f>'User Stories'!D28</f>
-        <v>As a  I can  so that .</v>
+        <v>As a System Administrator I can  so that .</v>
       </c>
       <c r="C28" s="28" t="str">
         <f>'User Stories'!E28</f>
         <v/>
       </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
     </row>
     <row r="29">
       <c r="A29" s="28" t="str">
         <f>'User Stories'!A29</f>
-        <v/>
+        <v>Test Center</v>
       </c>
       <c r="B29" s="28" t="str">
         <f>'User Stories'!D29</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Test Center I can  so that .</v>
       </c>
       <c r="C29" s="28" t="str">
         <f>'User Stories'!E29</f>
         <v/>
       </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
     </row>
     <row r="30">
       <c r="A30" s="28" t="str">
         <f>'User Stories'!A30</f>
-        <v/>
+        <v>Test Center</v>
       </c>
       <c r="B30" s="28" t="str">
         <f>'User Stories'!D30</f>
-        <v>As a  I can  so that .</v>
+        <v>As a Test Center I can  so that .</v>
       </c>
       <c r="C30" s="28" t="str">
         <f>'User Stories'!E30</f>
         <v/>
       </c>
-      <c r="D30" s="39"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
     </row>
     <row r="31">
       <c r="A31" s="28" t="str">
@@ -2657,11 +2823,11 @@
         <f>'User Stories'!E31</f>
         <v/>
       </c>
-      <c r="D31" s="39"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
     </row>
     <row r="32">
       <c r="A32" s="28" t="str">
@@ -2676,11 +2842,11 @@
         <f>'User Stories'!E32</f>
         <v/>
       </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
     </row>
     <row r="33">
       <c r="A33" s="28" t="str">
@@ -2695,11 +2861,11 @@
         <f>'User Stories'!E33</f>
         <v/>
       </c>
-      <c r="D33" s="39"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
     </row>
     <row r="34">
       <c r="A34" s="28" t="str">
@@ -2714,11 +2880,11 @@
         <f>'User Stories'!E34</f>
         <v/>
       </c>
-      <c r="D34" s="39"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
     </row>
     <row r="35">
       <c r="A35" s="28" t="str">
@@ -2733,11 +2899,11 @@
         <f>'User Stories'!E35</f>
         <v/>
       </c>
-      <c r="D35" s="39"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
     </row>
     <row r="36">
       <c r="A36" s="28" t="str">
@@ -2752,11 +2918,11 @@
         <f>'User Stories'!E36</f>
         <v/>
       </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
     </row>
     <row r="37">
       <c r="A37" s="28" t="str">
@@ -2771,11 +2937,11 @@
         <f>'User Stories'!E37</f>
         <v/>
       </c>
-      <c r="D37" s="39"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
     </row>
     <row r="38">
       <c r="A38" s="28" t="str">
@@ -2790,11 +2956,11 @@
         <f>'User Stories'!E37</f>
         <v/>
       </c>
-      <c r="D38" s="39"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
     </row>
     <row r="39">
       <c r="A39" s="28" t="str">
@@ -2809,11 +2975,11 @@
         <f>'User Stories'!E38</f>
         <v/>
       </c>
-      <c r="D39" s="39"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$2:$H$39">
@@ -2854,243 +3020,243 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="22" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>110</v>
+      <c r="A2" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>112</v>
+      <c r="A3" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>131</v>
       </c>
       <c r="C3" s="28"/>
-      <c r="D3" s="49">
+      <c r="D3" s="48">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="28"/>
-      <c r="D4" s="49">
+      <c r="D4" s="48">
         <v>3.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="50"/>
-      <c r="B5" s="51"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="28"/>
-      <c r="D5" s="49">
+      <c r="D5" s="48">
         <v>3.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="50"/>
-      <c r="B6" s="48" t="s">
-        <v>113</v>
+      <c r="A6" s="49"/>
+      <c r="B6" s="47" t="s">
+        <v>132</v>
       </c>
       <c r="C6" s="28"/>
-      <c r="D6" s="49">
+      <c r="D6" s="48">
         <v>5.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="28"/>
-      <c r="D7" s="49">
+      <c r="D7" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="28"/>
-      <c r="D8" s="49">
+      <c r="D8" s="48">
         <v>2.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="50"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="28"/>
-      <c r="D9" s="49">
+      <c r="D9" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="50"/>
-      <c r="B10" s="48" t="s">
-        <v>114</v>
+      <c r="A10" s="49"/>
+      <c r="B10" s="47" t="s">
+        <v>133</v>
       </c>
       <c r="C10" s="28"/>
-      <c r="D10" s="49">
+      <c r="D10" s="48">
         <v>5.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="28"/>
-      <c r="D11" s="49">
+      <c r="D11" s="48">
         <v>2.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="51"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="28"/>
-      <c r="D12" s="49">
+      <c r="D12" s="48">
         <v>1.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>116</v>
+      <c r="A13" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>135</v>
       </c>
       <c r="C13" s="28"/>
-      <c r="D13" s="49">
+      <c r="D13" s="48">
         <v>5.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="50"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="28"/>
-      <c r="D14" s="49">
+      <c r="D14" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="50"/>
-      <c r="B15" s="50"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="28"/>
-      <c r="D15" s="49">
+      <c r="D15" s="48">
         <v>1.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="50"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
-      <c r="D16" s="49">
+      <c r="D16" s="48">
         <v>1.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="50"/>
-      <c r="B17" s="51"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="28"/>
-      <c r="D17" s="49">
+      <c r="D17" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="50"/>
-      <c r="B18" s="48" t="s">
-        <v>117</v>
+      <c r="A18" s="49"/>
+      <c r="B18" s="47" t="s">
+        <v>136</v>
       </c>
       <c r="C18" s="28"/>
-      <c r="D18" s="49">
+      <c r="D18" s="48">
         <v>1.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="50"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
-      <c r="D19" s="49">
+      <c r="D19" s="48">
         <v>2.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="50"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="28"/>
-      <c r="D20" s="49">
+      <c r="D20" s="48">
         <v>2.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="28"/>
-      <c r="D21" s="49">
+      <c r="D21" s="48">
         <v>1.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="28"/>
-      <c r="D22" s="49">
+      <c r="D22" s="48">
         <v>3.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>119</v>
+      <c r="A23" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>138</v>
       </c>
       <c r="C23" s="28"/>
-      <c r="D23" s="49">
+      <c r="D23" s="48">
         <v>3.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="50"/>
-      <c r="B24" s="51"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="28"/>
-      <c r="D24" s="49">
+      <c r="D24" s="48">
         <v>5.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="48" t="s">
-        <v>120</v>
+      <c r="A25" s="49"/>
+      <c r="B25" s="47" t="s">
+        <v>139</v>
       </c>
       <c r="C25" s="28"/>
-      <c r="D25" s="49">
+      <c r="D25" s="48">
         <v>2.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="50"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="28"/>
-      <c r="D26" s="49">
+      <c r="D26" s="48">
         <v>0.5</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="51"/>
-      <c r="B27" s="51"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="28"/>
-      <c r="D27" s="49">
+      <c r="D27" s="48">
         <v>5.0</v>
       </c>
     </row>

</xml_diff>